<commit_message>
added joinTableEntity, deleted all collections from entities. refactor services.
</commit_message>
<xml_diff>
--- a/src/test/java/ru/fds/tavrzcms3/testdata/client_ind_new.xlsx
+++ b/src/test/java/ru/fds/tavrzcms3/testdata/client_ind_new.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <r>
       <t xml:space="preserve">client_manager_id: </t>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>2345 567890</t>
+  </si>
+  <si>
+    <t>Имя 3</t>
+  </si>
+  <si>
+    <t>Фамилия 2</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,6 +547,9 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
@@ -557,6 +566,9 @@
       </c>
       <c r="C4" t="s">
         <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>

</xml_diff>